<commit_message>
Implementada la persistencia para el cobro en MaquinaColectivo, falta hacer el Dao y ABM para poder probar el caso en el Main
</commit_message>
<xml_diff>
--- a/diagramas/CUs.xlsx
+++ b/diagramas/CUs.xlsx
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="56" uniqueCount="36">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="60" uniqueCount="40">
   <si>
     <t xml:space="preserve">numero de caso de uso</t>
   </si>
@@ -64,7 +64,7 @@
     <t xml:space="preserve">-</t>
   </si>
   <si>
-    <t xml:space="preserve">otorgarTarifaSocial</t>
+    <t xml:space="preserve">solicitarTarifaSocial</t>
   </si>
   <si>
     <t xml:space="preserve">pedir el beneficio de la tarifa social</t>
@@ -79,43 +79,55 @@
     <t xml:space="preserve">pedir el beneficio del boleto estudiantil</t>
   </si>
   <si>
+    <t xml:space="preserve">boletoEstudiantil: BoletoEstudiantil</t>
+  </si>
+  <si>
+    <t xml:space="preserve">MaquinaColectivo</t>
+  </si>
+  <si>
+    <t xml:space="preserve">cobrar</t>
+  </si>
+  <si>
+    <t xml:space="preserve">descuenta el valor del boleto (Colectivo)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">tarjeta: Tarjeta, boletoColectivo: BoletoColectivo</t>
+  </si>
+  <si>
+    <t xml:space="preserve">MaquinaTren</t>
+  </si>
+  <si>
+    <t xml:space="preserve">descuenta el valor del boleto (Tren)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Maquina</t>
+  </si>
+  <si>
+    <t xml:space="preserve">carga</t>
+  </si>
+  <si>
+    <t xml:space="preserve">recarga la tarjeta</t>
+  </si>
+  <si>
+    <t xml:space="preserve">float</t>
+  </si>
+  <si>
+    <t xml:space="preserve">devolverSaldo</t>
+  </si>
+  <si>
+    <t xml:space="preserve">devuelve el saldo al pasar por el molinete</t>
+  </si>
+  <si>
+    <t xml:space="preserve">SubeVirtual</t>
+  </si>
+  <si>
+    <t xml:space="preserve">calcularDescuento</t>
+  </si>
+  <si>
+    <t xml:space="preserve">calcula el descuento </t>
+  </si>
+  <si>
     <t xml:space="preserve">_</t>
-  </si>
-  <si>
-    <t xml:space="preserve">boolean</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Maquina</t>
-  </si>
-  <si>
-    <t xml:space="preserve">cobrar</t>
-  </si>
-  <si>
-    <t xml:space="preserve">descuenta el valor del boleto</t>
-  </si>
-  <si>
-    <t xml:space="preserve">carga</t>
-  </si>
-  <si>
-    <t xml:space="preserve">recarga la tarjeta</t>
-  </si>
-  <si>
-    <t xml:space="preserve">float</t>
-  </si>
-  <si>
-    <t xml:space="preserve">devolverSaldo</t>
-  </si>
-  <si>
-    <t xml:space="preserve">devuelve el saldo al pasar por el molinete</t>
-  </si>
-  <si>
-    <t xml:space="preserve">SubeVirtual</t>
-  </si>
-  <si>
-    <t xml:space="preserve">calcularDescuento</t>
-  </si>
-  <si>
-    <t xml:space="preserve">calcula el descuento </t>
   </si>
   <si>
     <t xml:space="preserve">BoletoTren</t>
@@ -311,10 +323,10 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:F11"/>
+  <dimension ref="A1:F12"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="B1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="E6" activeCellId="0" sqref="E6"/>
+      <selection pane="topLeft" activeCell="E8" activeCellId="0" sqref="E8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -426,7 +438,7 @@
         <v>19</v>
       </c>
       <c r="F5" s="3" t="s">
-        <v>20</v>
+        <v>10</v>
       </c>
     </row>
     <row r="6" s="2" customFormat="true" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -434,47 +446,45 @@
         <v>5</v>
       </c>
       <c r="B6" s="3" t="s">
+        <v>20</v>
+      </c>
+      <c r="C6" s="3" t="s">
         <v>21</v>
       </c>
-      <c r="C6" s="3" t="s">
+      <c r="D6" s="3" t="s">
         <v>22</v>
       </c>
-      <c r="D6" s="3" t="s">
+      <c r="E6" s="3" t="s">
         <v>23</v>
       </c>
-      <c r="E6" s="3" t="s">
-        <v>9</v>
-      </c>
       <c r="F6" s="3" t="s">
-        <v>20</v>
-      </c>
-    </row>
-    <row r="7" s="2" customFormat="true" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="7" s="2" customFormat="true" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A7" s="3" t="n">
         <v>6</v>
       </c>
       <c r="B7" s="3" t="s">
+        <v>24</v>
+      </c>
+      <c r="C7" s="3" t="s">
         <v>21</v>
-      </c>
-      <c r="C7" s="3" t="s">
-        <v>24</v>
       </c>
       <c r="D7" s="3" t="s">
         <v>25</v>
       </c>
-      <c r="E7" s="3" t="s">
-        <v>9</v>
-      </c>
+      <c r="E7" s="3"/>
       <c r="F7" s="3" t="s">
-        <v>26</v>
-      </c>
-    </row>
-    <row r="8" s="2" customFormat="true" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="8" s="2" customFormat="true" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A8" s="3" t="n">
         <v>7</v>
       </c>
       <c r="B8" s="3" t="s">
-        <v>21</v>
+        <v>26</v>
       </c>
       <c r="C8" s="3" t="s">
         <v>27</v>
@@ -486,15 +496,15 @@
         <v>9</v>
       </c>
       <c r="F8" s="3" t="s">
-        <v>26</v>
-      </c>
-    </row>
-    <row r="9" s="2" customFormat="true" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="9" s="2" customFormat="true" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A9" s="3" t="n">
         <v>8</v>
       </c>
       <c r="B9" s="3" t="s">
-        <v>29</v>
+        <v>26</v>
       </c>
       <c r="C9" s="3" t="s">
         <v>30</v>
@@ -503,13 +513,13 @@
         <v>31</v>
       </c>
       <c r="E9" s="3" t="s">
-        <v>19</v>
+        <v>9</v>
       </c>
       <c r="F9" s="3" t="s">
-        <v>26</v>
-      </c>
-    </row>
-    <row r="10" s="2" customFormat="true" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="10" s="2" customFormat="true" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A10" s="3" t="n">
         <v>9</v>
       </c>
@@ -523,28 +533,45 @@
         <v>34</v>
       </c>
       <c r="E10" s="3" t="s">
-        <v>19</v>
+        <v>35</v>
       </c>
       <c r="F10" s="3" t="s">
-        <v>26</v>
-      </c>
-    </row>
-    <row r="11" s="2" customFormat="true" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="11" s="2" customFormat="true" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A11" s="3"/>
       <c r="B11" s="3" t="s">
+        <v>36</v>
+      </c>
+      <c r="C11" s="3" t="s">
+        <v>37</v>
+      </c>
+      <c r="D11" s="3" t="s">
+        <v>38</v>
+      </c>
+      <c r="E11" s="3" t="s">
         <v>35</v>
       </c>
-      <c r="C11" s="3" t="s">
-        <v>33</v>
-      </c>
-      <c r="D11" s="3" t="s">
-        <v>34</v>
-      </c>
-      <c r="E11" s="3" t="s">
-        <v>19</v>
-      </c>
       <c r="F11" s="3" t="s">
-        <v>26</v>
+        <v>29</v>
+      </c>
+    </row>
+    <row r="12" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B12" s="3" t="s">
+        <v>39</v>
+      </c>
+      <c r="C12" s="3" t="s">
+        <v>37</v>
+      </c>
+      <c r="D12" s="3" t="s">
+        <v>38</v>
+      </c>
+      <c r="E12" s="3" t="s">
+        <v>35</v>
+      </c>
+      <c r="F12" s="3" t="s">
+        <v>29</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Caso de Uso Cobro en MaquinaColectivo andando
</commit_message>
<xml_diff>
--- a/diagramas/CUs.xlsx
+++ b/diagramas/CUs.xlsx
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="60" uniqueCount="40">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="59" uniqueCount="41">
   <si>
     <t xml:space="preserve">numero de caso de uso</t>
   </si>
@@ -91,7 +91,7 @@
     <t xml:space="preserve">descuenta el valor del boleto (Colectivo)</t>
   </si>
   <si>
-    <t xml:space="preserve">tarjeta: Tarjeta, boletoColectivo: BoletoColectivo</t>
+    <t xml:space="preserve">tarjeta: Tarjeta, boleto: Objeto</t>
   </si>
   <si>
     <t xml:space="preserve">MaquinaTren</t>
@@ -100,6 +100,15 @@
     <t xml:space="preserve">descuenta el valor del boleto (Tren)</t>
   </si>
   <si>
+    <t xml:space="preserve">devolverSaldo</t>
+  </si>
+  <si>
+    <t xml:space="preserve">devuelve el saldo al pasar por el molinete</t>
+  </si>
+  <si>
+    <t xml:space="preserve">float</t>
+  </si>
+  <si>
     <t xml:space="preserve">Maquina</t>
   </si>
   <si>
@@ -109,37 +118,31 @@
     <t xml:space="preserve">recarga la tarjeta</t>
   </si>
   <si>
-    <t xml:space="preserve">float</t>
-  </si>
-  <si>
-    <t xml:space="preserve">devolverSaldo</t>
-  </si>
-  <si>
-    <t xml:space="preserve">devuelve el saldo al pasar por el molinete</t>
-  </si>
-  <si>
-    <t xml:space="preserve">SubeVirtual</t>
+    <t xml:space="preserve">Casos integrados en otras funciones</t>
+  </si>
+  <si>
+    <t xml:space="preserve">BoletoColectivo</t>
+  </si>
+  <si>
+    <t xml:space="preserve">calcularValor</t>
+  </si>
+  <si>
+    <t xml:space="preserve">calcula el valor del boleto según la seccion – Integrado en cobrar (MaquinaColectivo)</t>
   </si>
   <si>
     <t xml:space="preserve">calcularDescuento</t>
   </si>
   <si>
-    <t xml:space="preserve">calcula el descuento </t>
+    <t xml:space="preserve">calcula el descuento – Integrado en cobrar (MaquinaColectivo)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">BoletoTren</t>
+  </si>
+  <si>
+    <t xml:space="preserve">calcula el valor del boleto según la seccion </t>
   </si>
   <si>
     <t xml:space="preserve">_</t>
-  </si>
-  <si>
-    <t xml:space="preserve">BoletoTren</t>
-  </si>
-  <si>
-    <t xml:space="preserve">calcularValor</t>
-  </si>
-  <si>
-    <t xml:space="preserve">calcula el valor del boleto según la seccion </t>
-  </si>
-  <si>
-    <t xml:space="preserve">BoletoColectivo</t>
   </si>
 </sst>
 </file>
@@ -229,7 +232,7 @@
     <xf numFmtId="42" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
   </cellStyleXfs>
-  <cellXfs count="4">
+  <cellXfs count="5">
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
@@ -244,6 +247,10 @@
     </xf>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="left" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
   </cellXfs>
@@ -323,10 +330,10 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:F12"/>
+  <dimension ref="A1:F21"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="B1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="E8" activeCellId="0" sqref="E8"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="B10" activeCellId="0" sqref="B10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -484,97 +491,123 @@
         <v>7</v>
       </c>
       <c r="B8" s="3" t="s">
+        <v>24</v>
+      </c>
+      <c r="C8" s="3" t="s">
         <v>26</v>
       </c>
-      <c r="C8" s="3" t="s">
+      <c r="D8" s="3" t="s">
         <v>27</v>
-      </c>
-      <c r="D8" s="3" t="s">
-        <v>28</v>
       </c>
       <c r="E8" s="3" t="s">
         <v>9</v>
       </c>
       <c r="F8" s="3" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
     </row>
     <row r="9" s="2" customFormat="true" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A9" s="3" t="n">
         <v>8</v>
       </c>
-      <c r="B9" s="3" t="s">
-        <v>26</v>
-      </c>
-      <c r="C9" s="3" t="s">
-        <v>30</v>
-      </c>
-      <c r="D9" s="3" t="s">
-        <v>31</v>
-      </c>
-      <c r="E9" s="3" t="s">
-        <v>9</v>
-      </c>
-      <c r="F9" s="3" t="s">
-        <v>29</v>
-      </c>
+      <c r="B9" s="0"/>
+      <c r="C9" s="0"/>
+      <c r="D9" s="0"/>
+      <c r="E9" s="0"/>
+      <c r="F9" s="0"/>
     </row>
     <row r="10" s="2" customFormat="true" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A10" s="3" t="n">
         <v>9</v>
       </c>
       <c r="B10" s="3" t="s">
-        <v>32</v>
+        <v>29</v>
       </c>
       <c r="C10" s="3" t="s">
-        <v>33</v>
+        <v>30</v>
       </c>
       <c r="D10" s="3" t="s">
-        <v>34</v>
+        <v>31</v>
       </c>
       <c r="E10" s="3" t="s">
-        <v>35</v>
+        <v>9</v>
       </c>
       <c r="F10" s="3" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
     </row>
     <row r="11" s="2" customFormat="true" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A11" s="3"/>
-      <c r="B11" s="3" t="s">
+      <c r="B11" s="0"/>
+      <c r="C11" s="0"/>
+      <c r="D11" s="0"/>
+      <c r="E11" s="0"/>
+      <c r="F11" s="0"/>
+    </row>
+    <row r="12" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="13" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="14" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="15" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A15" s="4" t="s">
+        <v>32</v>
+      </c>
+      <c r="B15" s="4"/>
+      <c r="C15" s="4"/>
+    </row>
+    <row r="16" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B16" s="3" t="s">
+        <v>33</v>
+      </c>
+      <c r="C16" s="3" t="s">
+        <v>34</v>
+      </c>
+      <c r="D16" s="4" t="s">
+        <v>35</v>
+      </c>
+      <c r="E16" s="4"/>
+      <c r="F16" s="3" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="17" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B17" s="3" t="s">
+        <v>20</v>
+      </c>
+      <c r="C17" s="3" t="s">
         <v>36</v>
       </c>
-      <c r="C11" s="3" t="s">
+      <c r="D17" s="3" t="s">
         <v>37</v>
       </c>
-      <c r="D11" s="3" t="s">
+      <c r="E17" s="3"/>
+      <c r="F17" s="3" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="18" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B18" s="3" t="s">
         <v>38</v>
       </c>
-      <c r="E11" s="3" t="s">
-        <v>35</v>
-      </c>
-      <c r="F11" s="3" t="s">
-        <v>29</v>
-      </c>
-    </row>
-    <row r="12" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B12" s="3" t="s">
+      <c r="C18" s="3" t="s">
+        <v>34</v>
+      </c>
+      <c r="D18" s="3" t="s">
         <v>39</v>
       </c>
-      <c r="C12" s="3" t="s">
-        <v>37</v>
-      </c>
-      <c r="D12" s="3" t="s">
-        <v>38</v>
-      </c>
-      <c r="E12" s="3" t="s">
-        <v>35</v>
-      </c>
-      <c r="F12" s="3" t="s">
-        <v>29</v>
-      </c>
-    </row>
+      <c r="E18" s="3" t="s">
+        <v>40</v>
+      </c>
+      <c r="F18" s="3" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="19" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="21" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
   </sheetData>
+  <mergeCells count="2">
+    <mergeCell ref="A15:C15"/>
+    <mergeCell ref="D16:E16"/>
+  </mergeCells>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.511805555555555" footer="0.511805555555555"/>
   <pageSetup paperSize="1" scale="100" firstPageNumber="0" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" blackAndWhite="false" draft="false" cellComments="none" useFirstPageNumber="false" horizontalDpi="300" verticalDpi="300" copies="1"/>

</xml_diff>

<commit_message>
Caso de uso Cobrar boleto en Tren andando y con persistencia, agregado el Dao, ABM, clase y mapeo para TarifaTren, modificado el DER y la el diagrama de clases para añadir TarifaTren, valor de la tarifa del tren puesto en una nueva tabla (TarifaTren) y puesto en BoletoTren con relacion
</commit_message>
<xml_diff>
--- a/diagramas/CUs.xlsx
+++ b/diagramas/CUs.xlsx
@@ -97,39 +97,42 @@
     <t xml:space="preserve">MaquinaTren</t>
   </si>
   <si>
+    <t xml:space="preserve">cobroMolinete</t>
+  </si>
+  <si>
     <t xml:space="preserve">descuenta el valor del boleto (Tren)</t>
   </si>
   <si>
-    <t xml:space="preserve">devolverSaldo</t>
-  </si>
-  <si>
-    <t xml:space="preserve">devuelve el saldo al pasar por el molinete</t>
+    <t xml:space="preserve">devolucionMolinete</t>
+  </si>
+  <si>
+    <t xml:space="preserve">devuelve la diferencia al pasar por el molinete de salida</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Maquina</t>
+  </si>
+  <si>
+    <t xml:space="preserve">carga</t>
+  </si>
+  <si>
+    <t xml:space="preserve">recarga la tarjeta</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Casos integrados en otras funciones</t>
+  </si>
+  <si>
+    <t xml:space="preserve">BoletoColectivo</t>
+  </si>
+  <si>
+    <t xml:space="preserve">calcularValor</t>
+  </si>
+  <si>
+    <t xml:space="preserve">calcula el valor del boleto según la seccion – Integrado en cobrar (MaquinaColectivo)</t>
   </si>
   <si>
     <t xml:space="preserve">float</t>
   </si>
   <si>
-    <t xml:space="preserve">Maquina</t>
-  </si>
-  <si>
-    <t xml:space="preserve">carga</t>
-  </si>
-  <si>
-    <t xml:space="preserve">recarga la tarjeta</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Casos integrados en otras funciones</t>
-  </si>
-  <si>
-    <t xml:space="preserve">BoletoColectivo</t>
-  </si>
-  <si>
-    <t xml:space="preserve">calcularValor</t>
-  </si>
-  <si>
-    <t xml:space="preserve">calcula el valor del boleto según la seccion – Integrado en cobrar (MaquinaColectivo)</t>
-  </si>
-  <si>
     <t xml:space="preserve">calcularDescuento</t>
   </si>
   <si>
@@ -139,10 +142,7 @@
     <t xml:space="preserve">BoletoTren</t>
   </si>
   <si>
-    <t xml:space="preserve">calcula el valor del boleto según la seccion </t>
-  </si>
-  <si>
-    <t xml:space="preserve">_</t>
+    <t xml:space="preserve">calcula el valor del boleto según la seccion – Integrado en cobroMolinete y devolucionMolinete (Tarjeta)</t>
   </si>
 </sst>
 </file>
@@ -333,7 +333,7 @@
   <dimension ref="A1:F21"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="B10" activeCellId="0" sqref="B10"/>
+      <selection pane="topLeft" activeCell="D18" activeCellId="0" sqref="D18"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -476,12 +476,14 @@
         <v>24</v>
       </c>
       <c r="C7" s="3" t="s">
-        <v>21</v>
+        <v>25</v>
       </c>
       <c r="D7" s="3" t="s">
-        <v>25</v>
-      </c>
-      <c r="E7" s="3"/>
+        <v>26</v>
+      </c>
+      <c r="E7" s="3" t="s">
+        <v>9</v>
+      </c>
       <c r="F7" s="3" t="s">
         <v>10</v>
       </c>
@@ -494,47 +496,47 @@
         <v>24</v>
       </c>
       <c r="C8" s="3" t="s">
-        <v>26</v>
+        <v>27</v>
       </c>
       <c r="D8" s="3" t="s">
-        <v>27</v>
+        <v>28</v>
       </c>
       <c r="E8" s="3" t="s">
         <v>9</v>
       </c>
       <c r="F8" s="3" t="s">
-        <v>28</v>
+        <v>10</v>
       </c>
     </row>
     <row r="9" s="2" customFormat="true" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A9" s="3" t="n">
         <v>8</v>
       </c>
-      <c r="B9" s="0"/>
-      <c r="C9" s="0"/>
-      <c r="D9" s="0"/>
-      <c r="E9" s="0"/>
-      <c r="F9" s="0"/>
+      <c r="B9" s="3" t="s">
+        <v>29</v>
+      </c>
+      <c r="C9" s="3" t="s">
+        <v>30</v>
+      </c>
+      <c r="D9" s="3" t="s">
+        <v>31</v>
+      </c>
+      <c r="E9" s="3" t="s">
+        <v>9</v>
+      </c>
+      <c r="F9" s="3" t="s">
+        <v>10</v>
+      </c>
     </row>
     <row r="10" s="2" customFormat="true" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A10" s="3" t="n">
         <v>9</v>
       </c>
-      <c r="B10" s="3" t="s">
-        <v>29</v>
-      </c>
-      <c r="C10" s="3" t="s">
-        <v>30</v>
-      </c>
-      <c r="D10" s="3" t="s">
-        <v>31</v>
-      </c>
-      <c r="E10" s="3" t="s">
-        <v>9</v>
-      </c>
-      <c r="F10" s="3" t="s">
-        <v>28</v>
-      </c>
+      <c r="B10" s="0"/>
+      <c r="C10" s="0"/>
+      <c r="D10" s="0"/>
+      <c r="E10" s="0"/>
+      <c r="F10" s="0"/>
     </row>
     <row r="11" s="2" customFormat="true" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A11" s="3"/>
@@ -566,7 +568,7 @@
       </c>
       <c r="E16" s="4"/>
       <c r="F16" s="3" t="s">
-        <v>28</v>
+        <v>36</v>
       </c>
     </row>
     <row r="17" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -574,39 +576,38 @@
         <v>20</v>
       </c>
       <c r="C17" s="3" t="s">
-        <v>36</v>
+        <v>37</v>
       </c>
       <c r="D17" s="3" t="s">
-        <v>37</v>
+        <v>38</v>
       </c>
       <c r="E17" s="3"/>
       <c r="F17" s="3" t="s">
-        <v>28</v>
+        <v>36</v>
       </c>
     </row>
     <row r="18" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B18" s="3" t="s">
-        <v>38</v>
+        <v>39</v>
       </c>
       <c r="C18" s="3" t="s">
         <v>34</v>
       </c>
-      <c r="D18" s="3" t="s">
-        <v>39</v>
-      </c>
-      <c r="E18" s="3" t="s">
+      <c r="D18" s="4" t="s">
         <v>40</v>
       </c>
+      <c r="E18" s="4"/>
       <c r="F18" s="3" t="s">
-        <v>28</v>
+        <v>36</v>
       </c>
     </row>
     <row r="19" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
     <row r="21" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
   </sheetData>
-  <mergeCells count="2">
+  <mergeCells count="3">
     <mergeCell ref="A15:C15"/>
     <mergeCell ref="D16:E16"/>
+    <mergeCell ref="D18:E18"/>
   </mergeCells>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.511805555555555" footer="0.511805555555555"/>

</xml_diff>

<commit_message>
Casos de Uso boleto de subte y carga, queda por implementar boleto estudiantil
</commit_message>
<xml_diff>
--- a/diagramas/CUs.xlsx
+++ b/diagramas/CUs.xlsx
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="59" uniqueCount="41">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="64" uniqueCount="43">
   <si>
     <t xml:space="preserve">numero de caso de uso</t>
   </si>
@@ -109,6 +109,12 @@
     <t xml:space="preserve">devuelve la diferencia al pasar por el molinete de salida</t>
   </si>
   <si>
+    <t xml:space="preserve">cobroMolineteSubte</t>
+  </si>
+  <si>
+    <t xml:space="preserve">descuenta el valor del boleto (Subte)</t>
+  </si>
+  <si>
     <t xml:space="preserve">Maquina</t>
   </si>
   <si>
@@ -118,6 +124,9 @@
     <t xml:space="preserve">recarga la tarjeta</t>
   </si>
   <si>
+    <t xml:space="preserve">tarjeta: Tarjeta, float: valor</t>
+  </si>
+  <si>
     <t xml:space="preserve">Casos integrados en otras funciones</t>
   </si>
   <si>
@@ -128,9 +137,6 @@
   </si>
   <si>
     <t xml:space="preserve">calcula el valor del boleto según la seccion – Integrado en cobrar (MaquinaColectivo)</t>
-  </si>
-  <si>
-    <t xml:space="preserve">float</t>
   </si>
   <si>
     <t xml:space="preserve">calcularDescuento</t>
@@ -249,7 +255,7 @@
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
       <alignment horizontal="left" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -333,7 +339,7 @@
   <dimension ref="A1:F21"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="D18" activeCellId="0" sqref="D18"/>
+      <selection pane="topLeft" activeCell="A19" activeCellId="0" sqref="A19"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -512,19 +518,19 @@
       <c r="A9" s="3" t="n">
         <v>8</v>
       </c>
-      <c r="B9" s="3" t="s">
+      <c r="B9" s="0" t="s">
+        <v>24</v>
+      </c>
+      <c r="C9" s="0" t="s">
         <v>29</v>
       </c>
-      <c r="C9" s="3" t="s">
+      <c r="D9" s="0" t="s">
         <v>30</v>
       </c>
-      <c r="D9" s="3" t="s">
-        <v>31</v>
-      </c>
-      <c r="E9" s="3" t="s">
+      <c r="E9" s="0" t="s">
         <v>9</v>
       </c>
-      <c r="F9" s="3" t="s">
+      <c r="F9" s="0" t="s">
         <v>10</v>
       </c>
     </row>
@@ -532,11 +538,21 @@
       <c r="A10" s="3" t="n">
         <v>9</v>
       </c>
-      <c r="B10" s="0"/>
-      <c r="C10" s="0"/>
-      <c r="D10" s="0"/>
-      <c r="E10" s="0"/>
-      <c r="F10" s="0"/>
+      <c r="B10" s="3" t="s">
+        <v>31</v>
+      </c>
+      <c r="C10" s="3" t="s">
+        <v>32</v>
+      </c>
+      <c r="D10" s="3" t="s">
+        <v>33</v>
+      </c>
+      <c r="E10" s="3" t="s">
+        <v>34</v>
+      </c>
+      <c r="F10" s="3" t="s">
+        <v>10</v>
+      </c>
     </row>
     <row r="11" s="2" customFormat="true" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A11" s="3"/>
@@ -551,24 +567,24 @@
     <row r="14" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
     <row r="15" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A15" s="4" t="s">
-        <v>32</v>
+        <v>35</v>
       </c>
       <c r="B15" s="4"/>
       <c r="C15" s="4"/>
     </row>
     <row r="16" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B16" s="3" t="s">
-        <v>33</v>
+        <v>36</v>
       </c>
       <c r="C16" s="3" t="s">
-        <v>34</v>
+        <v>37</v>
       </c>
       <c r="D16" s="4" t="s">
-        <v>35</v>
+        <v>38</v>
       </c>
       <c r="E16" s="4"/>
       <c r="F16" s="3" t="s">
-        <v>36</v>
+        <v>13</v>
       </c>
     </row>
     <row r="17" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -576,29 +592,29 @@
         <v>20</v>
       </c>
       <c r="C17" s="3" t="s">
-        <v>37</v>
+        <v>39</v>
       </c>
       <c r="D17" s="3" t="s">
-        <v>38</v>
+        <v>40</v>
       </c>
       <c r="E17" s="3"/>
       <c r="F17" s="3" t="s">
-        <v>36</v>
+        <v>13</v>
       </c>
     </row>
     <row r="18" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B18" s="3" t="s">
-        <v>39</v>
+        <v>41</v>
       </c>
       <c r="C18" s="3" t="s">
-        <v>34</v>
+        <v>37</v>
       </c>
       <c r="D18" s="4" t="s">
-        <v>40</v>
+        <v>42</v>
       </c>
       <c r="E18" s="4"/>
       <c r="F18" s="3" t="s">
-        <v>36</v>
+        <v>13</v>
       </c>
     </row>
     <row r="19" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>

</xml_diff>